<commit_message>
inputfield value modifieduser criterions
</commit_message>
<xml_diff>
--- a/criterion_property_definitions.xlsx
+++ b/criterion_property_definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\configuration\master-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C79185-E246-43E5-A953-35C6A6E6DBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86A9643-53EC-449C-950C-21472ECD83CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="27840" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="31395" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="criterion_property" sheetId="4" r:id="rId1"/>
@@ -19,11 +19,16 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="458">
   <si>
     <t>property</t>
   </si>
@@ -1385,6 +1390,18 @@
   </si>
   <si>
     <t>ctsms.VisitScheduleItem</t>
+  </si>
+  <si>
+    <t>IS_NULL, EQ, NE, GT, GE, LT, LE, LIKE, ILIKE</t>
+  </si>
+  <si>
+    <t>proband.inquiryValues.modifiedUser.id</t>
+  </si>
+  <si>
+    <t>proband.trialParticipations.tagValues.modifiedUser.id</t>
+  </si>
+  <si>
+    <t>proband.trialParticipations.ecrfValues.modifiedUser.id</t>
   </si>
 </sst>
 </file>
@@ -1761,10 +1778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M302"/>
+  <dimension ref="A1:M305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F283" workbookViewId="0">
-      <selection activeCell="L292" sqref="L292"/>
+    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
+      <selection activeCell="M241" sqref="M241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4490,7 +4507,7 @@
         <v>375</v>
       </c>
       <c r="M138" t="s">
-        <v>122</v>
+        <v>454</v>
       </c>
     </row>
     <row r="139" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4564,7 +4581,7 @@
         <v>376</v>
       </c>
       <c r="M142" t="s">
-        <v>122</v>
+        <v>454</v>
       </c>
     </row>
     <row r="143" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5564,19 +5581,19 @@
         <v>77</v>
       </c>
       <c r="B192" t="s">
-        <v>133</v>
+        <v>455</v>
       </c>
       <c r="C192" t="s">
-        <v>15</v>
-      </c>
-      <c r="H192" t="s">
-        <v>132</v>
+        <v>9</v>
+      </c>
+      <c r="K192" t="s">
+        <v>114</v>
       </c>
       <c r="L192" t="s">
-        <v>133</v>
+        <v>455</v>
       </c>
       <c r="M192" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="193" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5584,16 +5601,19 @@
         <v>77</v>
       </c>
       <c r="B193" t="s">
-        <v>91</v>
+        <v>133</v>
       </c>
       <c r="C193" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="H193" t="s">
+        <v>132</v>
       </c>
       <c r="L193" t="s">
-        <v>91</v>
+        <v>133</v>
       </c>
       <c r="M193" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="194" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5601,16 +5621,16 @@
         <v>77</v>
       </c>
       <c r="B194" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C194" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="L194" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M194" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="195" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5618,13 +5638,13 @@
         <v>77</v>
       </c>
       <c r="B195" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C195" t="s">
-        <v>94</v>
+        <v>9</v>
       </c>
       <c r="L195" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M195" t="s">
         <v>127</v>
@@ -5635,13 +5655,13 @@
         <v>77</v>
       </c>
       <c r="B196" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C196" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="L196" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M196" t="s">
         <v>127</v>
@@ -5655,19 +5675,13 @@
         <v>95</v>
       </c>
       <c r="C197" t="s">
-        <v>15</v>
-      </c>
-      <c r="D197" t="s">
-        <v>308</v>
-      </c>
-      <c r="J197" t="s">
-        <v>438</v>
+        <v>33</v>
       </c>
       <c r="L197" t="s">
-        <v>231</v>
-      </c>
-      <c r="M197" s="1" t="s">
-        <v>244</v>
+        <v>95</v>
+      </c>
+      <c r="M197" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="198" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5675,16 +5689,22 @@
         <v>77</v>
       </c>
       <c r="B198" t="s">
-        <v>192</v>
+        <v>95</v>
       </c>
       <c r="C198" t="s">
-        <v>52</v>
+        <v>15</v>
+      </c>
+      <c r="D198" t="s">
+        <v>308</v>
+      </c>
+      <c r="J198" t="s">
+        <v>438</v>
       </c>
       <c r="L198" t="s">
-        <v>192</v>
-      </c>
-      <c r="M198" t="s">
-        <v>127</v>
+        <v>231</v>
+      </c>
+      <c r="M198" s="1" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="199" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5695,19 +5715,13 @@
         <v>192</v>
       </c>
       <c r="C199" t="s">
-        <v>15</v>
-      </c>
-      <c r="D199" t="s">
-        <v>308</v>
-      </c>
-      <c r="J199" t="s">
-        <v>438</v>
+        <v>52</v>
       </c>
       <c r="L199" t="s">
-        <v>230</v>
-      </c>
-      <c r="M199" s="1" t="s">
-        <v>245</v>
+        <v>192</v>
+      </c>
+      <c r="M199" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="200" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5715,16 +5729,22 @@
         <v>77</v>
       </c>
       <c r="B200" t="s">
-        <v>287</v>
+        <v>192</v>
       </c>
       <c r="C200" t="s">
-        <v>284</v>
+        <v>15</v>
+      </c>
+      <c r="D200" t="s">
+        <v>308</v>
+      </c>
+      <c r="J200" t="s">
+        <v>438</v>
       </c>
       <c r="L200" t="s">
-        <v>287</v>
-      </c>
-      <c r="M200" t="s">
-        <v>127</v>
+        <v>230</v>
+      </c>
+      <c r="M200" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="201" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5735,47 +5755,35 @@
         <v>287</v>
       </c>
       <c r="C201" t="s">
-        <v>9</v>
+        <v>284</v>
       </c>
       <c r="L201" t="s">
-        <v>288</v>
-      </c>
-      <c r="M201" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
+      </c>
+      <c r="M201" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="202" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>180</v>
+        <v>77</v>
       </c>
       <c r="B202" t="s">
-        <v>96</v>
+        <v>287</v>
       </c>
       <c r="C202" t="s">
         <v>9</v>
       </c>
-      <c r="D202" t="s">
-        <v>327</v>
-      </c>
-      <c r="E202" t="s">
-        <v>97</v>
-      </c>
-      <c r="F202" t="s">
-        <v>88</v>
-      </c>
-      <c r="G202" t="s">
-        <v>12</v>
-      </c>
       <c r="L202" t="s">
-        <v>96</v>
-      </c>
-      <c r="M202" t="s">
-        <v>121</v>
+        <v>288</v>
+      </c>
+      <c r="M202" s="1" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="203" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>77</v>
+        <v>180</v>
       </c>
       <c r="B203" t="s">
         <v>96</v>
@@ -5786,14 +5794,14 @@
       <c r="D203" t="s">
         <v>327</v>
       </c>
+      <c r="E203" t="s">
+        <v>97</v>
+      </c>
       <c r="F203" t="s">
         <v>88</v>
       </c>
-      <c r="H203" t="s">
-        <v>273</v>
-      </c>
-      <c r="I203" t="s">
-        <v>274</v>
+      <c r="G203" t="s">
+        <v>12</v>
       </c>
       <c r="L203" t="s">
         <v>96</v>
@@ -5807,19 +5815,28 @@
         <v>77</v>
       </c>
       <c r="B204" t="s">
-        <v>141</v>
+        <v>96</v>
       </c>
       <c r="C204" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="D204" t="s">
+        <v>327</v>
+      </c>
+      <c r="F204" t="s">
+        <v>88</v>
       </c>
       <c r="H204" t="s">
-        <v>410</v>
+        <v>273</v>
+      </c>
+      <c r="I204" t="s">
+        <v>274</v>
       </c>
       <c r="L204" t="s">
-        <v>141</v>
+        <v>96</v>
       </c>
       <c r="M204" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="205" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5827,50 +5844,41 @@
         <v>77</v>
       </c>
       <c r="B205" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C205" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="H205" t="s">
+        <v>410</v>
       </c>
       <c r="L205" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="M205" t="s">
-        <v>449</v>
+        <v>122</v>
       </c>
     </row>
     <row r="206" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>180</v>
+        <v>77</v>
       </c>
       <c r="B206" t="s">
-        <v>98</v>
+        <v>136</v>
       </c>
       <c r="C206" t="s">
         <v>9</v>
       </c>
-      <c r="D206" t="s">
-        <v>328</v>
-      </c>
-      <c r="E206" t="s">
-        <v>99</v>
-      </c>
-      <c r="F206" t="s">
-        <v>88</v>
-      </c>
-      <c r="G206" t="s">
-        <v>12</v>
-      </c>
       <c r="L206" t="s">
-        <v>98</v>
+        <v>136</v>
       </c>
       <c r="M206" t="s">
-        <v>121</v>
+        <v>449</v>
       </c>
     </row>
     <row r="207" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>77</v>
+        <v>180</v>
       </c>
       <c r="B207" t="s">
         <v>98</v>
@@ -5881,14 +5889,14 @@
       <c r="D207" t="s">
         <v>328</v>
       </c>
+      <c r="E207" t="s">
+        <v>99</v>
+      </c>
       <c r="F207" t="s">
         <v>88</v>
       </c>
-      <c r="H207" t="s">
-        <v>275</v>
-      </c>
-      <c r="I207" t="s">
-        <v>276</v>
+      <c r="G207" t="s">
+        <v>12</v>
       </c>
       <c r="L207" t="s">
         <v>98</v>
@@ -5899,28 +5907,28 @@
     </row>
     <row r="208" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>180</v>
+        <v>77</v>
       </c>
       <c r="B208" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C208" t="s">
         <v>9</v>
       </c>
       <c r="D208" t="s">
-        <v>326</v>
-      </c>
-      <c r="E208" t="s">
-        <v>101</v>
+        <v>328</v>
       </c>
       <c r="F208" t="s">
-        <v>11</v>
-      </c>
-      <c r="G208" t="s">
-        <v>12</v>
+        <v>88</v>
+      </c>
+      <c r="H208" t="s">
+        <v>275</v>
+      </c>
+      <c r="I208" t="s">
+        <v>276</v>
       </c>
       <c r="L208" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="M208" t="s">
         <v>121</v>
@@ -5928,7 +5936,7 @@
     </row>
     <row r="209" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>77</v>
+        <v>180</v>
       </c>
       <c r="B209" t="s">
         <v>100</v>
@@ -5939,14 +5947,14 @@
       <c r="D209" t="s">
         <v>326</v>
       </c>
+      <c r="E209" t="s">
+        <v>101</v>
+      </c>
       <c r="F209" t="s">
         <v>11</v>
       </c>
-      <c r="H209" t="s">
-        <v>277</v>
-      </c>
-      <c r="I209" t="s">
-        <v>272</v>
+      <c r="G209" t="s">
+        <v>12</v>
       </c>
       <c r="L209" t="s">
         <v>100</v>
@@ -5960,53 +5968,65 @@
         <v>77</v>
       </c>
       <c r="B210" t="s">
-        <v>178</v>
+        <v>100</v>
       </c>
       <c r="C210" t="s">
         <v>9</v>
       </c>
+      <c r="D210" t="s">
+        <v>326</v>
+      </c>
+      <c r="F210" t="s">
+        <v>11</v>
+      </c>
+      <c r="H210" t="s">
+        <v>277</v>
+      </c>
+      <c r="I210" t="s">
+        <v>272</v>
+      </c>
       <c r="L210" t="s">
-        <v>178</v>
+        <v>100</v>
       </c>
       <c r="M210" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="211" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>180</v>
+        <v>77</v>
       </c>
       <c r="B211" t="s">
-        <v>112</v>
+        <v>178</v>
       </c>
       <c r="C211" t="s">
         <v>9</v>
       </c>
-      <c r="K211" t="s">
-        <v>39</v>
-      </c>
       <c r="L211" t="s">
-        <v>112</v>
+        <v>178</v>
       </c>
       <c r="M211" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="212" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>77</v>
+        <v>180</v>
       </c>
       <c r="B212" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="C212" t="s">
-        <v>52</v>
+        <v>9</v>
+      </c>
+      <c r="K212" t="s">
+        <v>39</v>
       </c>
       <c r="L212" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="M212" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="213" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6017,19 +6037,13 @@
         <v>130</v>
       </c>
       <c r="C213" t="s">
-        <v>15</v>
-      </c>
-      <c r="D213" t="s">
-        <v>308</v>
-      </c>
-      <c r="J213" t="s">
-        <v>438</v>
+        <v>52</v>
       </c>
       <c r="L213" t="s">
-        <v>229</v>
-      </c>
-      <c r="M213" s="1" t="s">
-        <v>245</v>
+        <v>130</v>
+      </c>
+      <c r="M213" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="214" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6037,19 +6051,22 @@
         <v>77</v>
       </c>
       <c r="B214" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C214" t="s">
         <v>15</v>
       </c>
-      <c r="H214" t="s">
-        <v>132</v>
+      <c r="D214" t="s">
+        <v>308</v>
+      </c>
+      <c r="J214" t="s">
+        <v>438</v>
       </c>
       <c r="L214" t="s">
-        <v>134</v>
-      </c>
-      <c r="M214" t="s">
-        <v>122</v>
+        <v>229</v>
+      </c>
+      <c r="M214" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="215" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6057,13 +6074,16 @@
         <v>77</v>
       </c>
       <c r="B215" t="s">
-        <v>102</v>
+        <v>456</v>
       </c>
       <c r="C215" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="K215" t="s">
+        <v>114</v>
       </c>
       <c r="L215" t="s">
-        <v>102</v>
+        <v>456</v>
       </c>
       <c r="M215" t="s">
         <v>121</v>
@@ -6074,16 +6094,19 @@
         <v>77</v>
       </c>
       <c r="B216" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
       <c r="C216" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="H216" t="s">
+        <v>132</v>
       </c>
       <c r="L216" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
       <c r="M216" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="217" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6091,16 +6114,16 @@
         <v>77</v>
       </c>
       <c r="B217" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C217" t="s">
-        <v>94</v>
+        <v>17</v>
       </c>
       <c r="L217" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M217" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="218" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6108,13 +6131,13 @@
         <v>77</v>
       </c>
       <c r="B218" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C218" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="L218" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M218" t="s">
         <v>127</v>
@@ -6125,22 +6148,16 @@
         <v>77</v>
       </c>
       <c r="B219" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C219" t="s">
-        <v>15</v>
-      </c>
-      <c r="D219" t="s">
-        <v>308</v>
-      </c>
-      <c r="J219" t="s">
-        <v>438</v>
+        <v>94</v>
       </c>
       <c r="L219" t="s">
-        <v>228</v>
-      </c>
-      <c r="M219" s="1" t="s">
-        <v>244</v>
+        <v>104</v>
+      </c>
+      <c r="M219" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="220" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6148,13 +6165,13 @@
         <v>77</v>
       </c>
       <c r="B220" t="s">
-        <v>191</v>
+        <v>105</v>
       </c>
       <c r="C220" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="L220" t="s">
-        <v>191</v>
+        <v>105</v>
       </c>
       <c r="M220" t="s">
         <v>127</v>
@@ -6165,7 +6182,7 @@
         <v>77</v>
       </c>
       <c r="B221" t="s">
-        <v>191</v>
+        <v>105</v>
       </c>
       <c r="C221" t="s">
         <v>15</v>
@@ -6177,10 +6194,10 @@
         <v>438</v>
       </c>
       <c r="L221" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="M221" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="222" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6188,13 +6205,13 @@
         <v>77</v>
       </c>
       <c r="B222" t="s">
-        <v>290</v>
+        <v>191</v>
       </c>
       <c r="C222" t="s">
-        <v>284</v>
+        <v>52</v>
       </c>
       <c r="L222" t="s">
-        <v>290</v>
+        <v>191</v>
       </c>
       <c r="M222" t="s">
         <v>127</v>
@@ -6205,45 +6222,39 @@
         <v>77</v>
       </c>
       <c r="B223" t="s">
-        <v>290</v>
+        <v>191</v>
       </c>
       <c r="C223" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="D223" t="s">
+        <v>308</v>
+      </c>
+      <c r="J223" t="s">
+        <v>438</v>
       </c>
       <c r="L223" t="s">
-        <v>291</v>
+        <v>227</v>
       </c>
       <c r="M223" s="1" t="s">
-        <v>289</v>
+        <v>245</v>
       </c>
     </row>
     <row r="224" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>180</v>
+        <v>77</v>
       </c>
       <c r="B224" t="s">
-        <v>106</v>
+        <v>290</v>
       </c>
       <c r="C224" t="s">
-        <v>9</v>
-      </c>
-      <c r="D224" t="s">
-        <v>327</v>
-      </c>
-      <c r="E224" t="s">
-        <v>107</v>
-      </c>
-      <c r="F224" t="s">
-        <v>88</v>
-      </c>
-      <c r="G224" t="s">
-        <v>12</v>
+        <v>284</v>
       </c>
       <c r="L224" t="s">
-        <v>106</v>
+        <v>290</v>
       </c>
       <c r="M224" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="225" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6251,48 +6262,45 @@
         <v>77</v>
       </c>
       <c r="B225" t="s">
-        <v>106</v>
+        <v>290</v>
       </c>
       <c r="C225" t="s">
         <v>9</v>
       </c>
-      <c r="D225" t="s">
-        <v>327</v>
-      </c>
-      <c r="F225" t="s">
-        <v>88</v>
-      </c>
-      <c r="H225" t="s">
-        <v>278</v>
-      </c>
-      <c r="I225" t="s">
-        <v>274</v>
-      </c>
       <c r="L225" t="s">
-        <v>106</v>
-      </c>
-      <c r="M225" t="s">
-        <v>121</v>
+        <v>291</v>
+      </c>
+      <c r="M225" s="1" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="226" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>77</v>
+        <v>180</v>
       </c>
       <c r="B226" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="C226" t="s">
-        <v>15</v>
-      </c>
-      <c r="H226" t="s">
-        <v>410</v>
+        <v>9</v>
+      </c>
+      <c r="D226" t="s">
+        <v>327</v>
+      </c>
+      <c r="E226" t="s">
+        <v>107</v>
+      </c>
+      <c r="F226" t="s">
+        <v>88</v>
+      </c>
+      <c r="G226" t="s">
+        <v>12</v>
       </c>
       <c r="L226" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="M226" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="227" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6300,16 +6308,28 @@
         <v>77</v>
       </c>
       <c r="B227" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="C227" t="s">
         <v>9</v>
       </c>
+      <c r="D227" t="s">
+        <v>327</v>
+      </c>
+      <c r="F227" t="s">
+        <v>88</v>
+      </c>
+      <c r="H227" t="s">
+        <v>278</v>
+      </c>
+      <c r="I227" t="s">
+        <v>274</v>
+      </c>
       <c r="L227" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="M227" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="228" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6317,16 +6337,19 @@
         <v>77</v>
       </c>
       <c r="B228" t="s">
-        <v>108</v>
+        <v>142</v>
       </c>
       <c r="C228" t="s">
-        <v>81</v>
+        <v>15</v>
+      </c>
+      <c r="H228" t="s">
+        <v>410</v>
       </c>
       <c r="L228" t="s">
-        <v>108</v>
+        <v>142</v>
       </c>
       <c r="M228" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="229" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6334,28 +6357,16 @@
         <v>77</v>
       </c>
       <c r="B229" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="C229" t="s">
         <v>9</v>
       </c>
-      <c r="D229" t="s">
-        <v>333</v>
-      </c>
-      <c r="E229" t="s">
-        <v>110</v>
-      </c>
-      <c r="F229" t="s">
-        <v>11</v>
-      </c>
-      <c r="G229" t="s">
-        <v>12</v>
-      </c>
       <c r="L229" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="M229" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="230" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6363,42 +6374,42 @@
         <v>77</v>
       </c>
       <c r="B230" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C230" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="L230" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="M230" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="231" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>180</v>
+        <v>77</v>
       </c>
       <c r="B231" t="s">
-        <v>334</v>
+        <v>109</v>
       </c>
       <c r="C231" t="s">
         <v>9</v>
       </c>
       <c r="D231" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E231" t="s">
-        <v>336</v>
+        <v>110</v>
       </c>
       <c r="F231" t="s">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="G231" t="s">
         <v>12</v>
       </c>
       <c r="L231" t="s">
-        <v>334</v>
+        <v>109</v>
       </c>
       <c r="M231" t="s">
         <v>121</v>
@@ -6409,28 +6420,16 @@
         <v>77</v>
       </c>
       <c r="B232" t="s">
-        <v>334</v>
+        <v>111</v>
       </c>
       <c r="C232" t="s">
         <v>9</v>
       </c>
-      <c r="D232" t="s">
-        <v>335</v>
-      </c>
-      <c r="F232" t="s">
-        <v>88</v>
-      </c>
-      <c r="H232" t="s">
-        <v>337</v>
-      </c>
-      <c r="I232" t="s">
-        <v>338</v>
-      </c>
       <c r="L232" t="s">
-        <v>334</v>
+        <v>111</v>
       </c>
       <c r="M232" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="233" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6438,25 +6437,25 @@
         <v>180</v>
       </c>
       <c r="B233" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="C233" t="s">
         <v>9</v>
       </c>
       <c r="D233" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
       <c r="E233" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="F233" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="G233" t="s">
         <v>12</v>
       </c>
       <c r="L233" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="M233" t="s">
         <v>121</v>
@@ -6467,25 +6466,25 @@
         <v>77</v>
       </c>
       <c r="B234" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="C234" t="s">
         <v>9</v>
       </c>
       <c r="D234" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
       <c r="F234" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="H234" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="I234" t="s">
-        <v>272</v>
+        <v>338</v>
       </c>
       <c r="L234" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="M234" t="s">
         <v>121</v>
@@ -6493,36 +6492,57 @@
     </row>
     <row r="235" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>77</v>
+        <v>180</v>
       </c>
       <c r="B235" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C235" t="s">
         <v>9</v>
       </c>
+      <c r="D235" t="s">
+        <v>326</v>
+      </c>
+      <c r="E235" t="s">
+        <v>340</v>
+      </c>
+      <c r="F235" t="s">
+        <v>11</v>
+      </c>
+      <c r="G235" t="s">
+        <v>12</v>
+      </c>
       <c r="L235" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="M235" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="236" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>180</v>
+        <v>77</v>
       </c>
       <c r="B236" t="s">
-        <v>112</v>
+        <v>339</v>
       </c>
       <c r="C236" t="s">
         <v>9</v>
       </c>
-      <c r="K236" t="s">
-        <v>39</v>
+      <c r="D236" t="s">
+        <v>326</v>
+      </c>
+      <c r="F236" t="s">
+        <v>11</v>
+      </c>
+      <c r="H236" t="s">
+        <v>341</v>
+      </c>
+      <c r="I236" t="s">
+        <v>272</v>
       </c>
       <c r="L236" t="s">
-        <v>112</v>
+        <v>339</v>
       </c>
       <c r="M236" t="s">
         <v>121</v>
@@ -6533,39 +6553,36 @@
         <v>77</v>
       </c>
       <c r="B237" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C237" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="L237" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="M237" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="238" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>77</v>
+        <v>180</v>
       </c>
       <c r="B238" t="s">
-        <v>343</v>
+        <v>112</v>
       </c>
       <c r="C238" t="s">
-        <v>15</v>
-      </c>
-      <c r="D238" t="s">
-        <v>308</v>
-      </c>
-      <c r="J238" t="s">
-        <v>438</v>
+        <v>9</v>
+      </c>
+      <c r="K238" t="s">
+        <v>39</v>
       </c>
       <c r="L238" t="s">
-        <v>344</v>
-      </c>
-      <c r="M238" s="1" t="s">
-        <v>245</v>
+        <v>112</v>
+      </c>
+      <c r="M238" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="239" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6573,19 +6590,16 @@
         <v>77</v>
       </c>
       <c r="B239" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C239" t="s">
-        <v>15</v>
-      </c>
-      <c r="H239" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="L239" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="M239" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="240" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6593,16 +6607,22 @@
         <v>77</v>
       </c>
       <c r="B240" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C240" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="D240" t="s">
+        <v>308</v>
+      </c>
+      <c r="J240" t="s">
+        <v>438</v>
       </c>
       <c r="L240" t="s">
-        <v>346</v>
-      </c>
-      <c r="M240" t="s">
-        <v>121</v>
+        <v>344</v>
+      </c>
+      <c r="M240" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="241" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6610,16 +6630,19 @@
         <v>77</v>
       </c>
       <c r="B241" t="s">
-        <v>347</v>
+        <v>457</v>
       </c>
       <c r="C241" t="s">
         <v>9</v>
       </c>
+      <c r="K241" t="s">
+        <v>114</v>
+      </c>
       <c r="L241" t="s">
-        <v>347</v>
+        <v>457</v>
       </c>
       <c r="M241" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="242" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6627,16 +6650,19 @@
         <v>77</v>
       </c>
       <c r="B242" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C242" t="s">
-        <v>94</v>
+        <v>15</v>
+      </c>
+      <c r="H242" t="s">
+        <v>132</v>
       </c>
       <c r="L242" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="M242" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="243" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6644,16 +6670,16 @@
         <v>77</v>
       </c>
       <c r="B243" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C243" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="L243" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="M243" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="244" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6661,22 +6687,16 @@
         <v>77</v>
       </c>
       <c r="B244" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C244" t="s">
-        <v>15</v>
-      </c>
-      <c r="D244" t="s">
-        <v>308</v>
-      </c>
-      <c r="J244" t="s">
-        <v>438</v>
+        <v>9</v>
       </c>
       <c r="L244" t="s">
-        <v>350</v>
-      </c>
-      <c r="M244" s="1" t="s">
-        <v>244</v>
+        <v>347</v>
+      </c>
+      <c r="M244" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="245" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6684,13 +6704,13 @@
         <v>77</v>
       </c>
       <c r="B245" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C245" t="s">
-        <v>52</v>
+        <v>94</v>
       </c>
       <c r="L245" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="M245" t="s">
         <v>127</v>
@@ -6701,22 +6721,16 @@
         <v>77</v>
       </c>
       <c r="B246" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C246" t="s">
-        <v>15</v>
-      </c>
-      <c r="D246" t="s">
-        <v>308</v>
-      </c>
-      <c r="J246" t="s">
-        <v>438</v>
+        <v>33</v>
       </c>
       <c r="L246" t="s">
-        <v>352</v>
-      </c>
-      <c r="M246" s="1" t="s">
-        <v>245</v>
+        <v>349</v>
+      </c>
+      <c r="M246" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="247" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6724,16 +6738,22 @@
         <v>77</v>
       </c>
       <c r="B247" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C247" t="s">
-        <v>284</v>
+        <v>15</v>
+      </c>
+      <c r="D247" t="s">
+        <v>308</v>
+      </c>
+      <c r="J247" t="s">
+        <v>438</v>
       </c>
       <c r="L247" t="s">
-        <v>353</v>
-      </c>
-      <c r="M247" t="s">
-        <v>127</v>
+        <v>350</v>
+      </c>
+      <c r="M247" s="1" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="248" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6741,45 +6761,39 @@
         <v>77</v>
       </c>
       <c r="B248" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C248" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="L248" t="s">
-        <v>354</v>
-      </c>
-      <c r="M248" s="1" t="s">
-        <v>289</v>
+        <v>351</v>
+      </c>
+      <c r="M248" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="249" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>180</v>
+        <v>77</v>
       </c>
       <c r="B249" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C249" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D249" t="s">
-        <v>327</v>
-      </c>
-      <c r="E249" t="s">
-        <v>358</v>
-      </c>
-      <c r="F249" t="s">
-        <v>88</v>
-      </c>
-      <c r="G249" t="s">
-        <v>12</v>
+        <v>308</v>
+      </c>
+      <c r="J249" t="s">
+        <v>438</v>
       </c>
       <c r="L249" t="s">
-        <v>355</v>
-      </c>
-      <c r="M249" t="s">
-        <v>121</v>
+        <v>352</v>
+      </c>
+      <c r="M249" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="250" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6787,28 +6801,16 @@
         <v>77</v>
       </c>
       <c r="B250" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C250" t="s">
-        <v>9</v>
-      </c>
-      <c r="D250" t="s">
-        <v>327</v>
-      </c>
-      <c r="F250" t="s">
-        <v>88</v>
-      </c>
-      <c r="H250" t="s">
-        <v>359</v>
-      </c>
-      <c r="I250" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="L250" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="M250" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="251" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6816,36 +6818,45 @@
         <v>77</v>
       </c>
       <c r="B251" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C251" t="s">
-        <v>15</v>
-      </c>
-      <c r="H251" t="s">
-        <v>410</v>
+        <v>9</v>
       </c>
       <c r="L251" t="s">
-        <v>356</v>
-      </c>
-      <c r="M251" t="s">
-        <v>122</v>
+        <v>354</v>
+      </c>
+      <c r="M251" s="1" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="252" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>77</v>
+        <v>180</v>
       </c>
       <c r="B252" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C252" t="s">
         <v>9</v>
       </c>
+      <c r="D252" t="s">
+        <v>327</v>
+      </c>
+      <c r="E252" t="s">
+        <v>358</v>
+      </c>
+      <c r="F252" t="s">
+        <v>88</v>
+      </c>
+      <c r="G252" t="s">
+        <v>12</v>
+      </c>
       <c r="L252" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="M252" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="253" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6853,13 +6864,25 @@
         <v>77</v>
       </c>
       <c r="B253" t="s">
-        <v>150</v>
+        <v>355</v>
       </c>
       <c r="C253" t="s">
-        <v>81</v>
+        <v>9</v>
+      </c>
+      <c r="D253" t="s">
+        <v>327</v>
+      </c>
+      <c r="F253" t="s">
+        <v>88</v>
+      </c>
+      <c r="H253" t="s">
+        <v>359</v>
+      </c>
+      <c r="I253" t="s">
+        <v>274</v>
       </c>
       <c r="L253" t="s">
-        <v>150</v>
+        <v>355</v>
       </c>
       <c r="M253" t="s">
         <v>121</v>
@@ -6870,22 +6893,19 @@
         <v>77</v>
       </c>
       <c r="B254" t="s">
-        <v>151</v>
+        <v>356</v>
       </c>
       <c r="C254" t="s">
-        <v>9</v>
-      </c>
-      <c r="D254" t="s">
-        <v>314</v>
-      </c>
-      <c r="J254" t="s">
-        <v>430</v>
+        <v>15</v>
+      </c>
+      <c r="H254" t="s">
+        <v>410</v>
       </c>
       <c r="L254" t="s">
-        <v>151</v>
+        <v>356</v>
       </c>
       <c r="M254" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="255" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6893,13 +6913,13 @@
         <v>77</v>
       </c>
       <c r="B255" t="s">
-        <v>152</v>
+        <v>357</v>
       </c>
       <c r="C255" t="s">
         <v>9</v>
       </c>
       <c r="L255" t="s">
-        <v>152</v>
+        <v>357</v>
       </c>
       <c r="M255" t="s">
         <v>125</v>
@@ -6910,13 +6930,13 @@
         <v>77</v>
       </c>
       <c r="B256" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C256" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="L256" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="M256" t="s">
         <v>121</v>
@@ -6927,16 +6947,19 @@
         <v>77</v>
       </c>
       <c r="B257" t="s">
-        <v>405</v>
+        <v>151</v>
       </c>
       <c r="C257" t="s">
         <v>9</v>
       </c>
-      <c r="K257" t="s">
-        <v>385</v>
+      <c r="D257" t="s">
+        <v>314</v>
+      </c>
+      <c r="J257" t="s">
+        <v>430</v>
       </c>
       <c r="L257" t="s">
-        <v>405</v>
+        <v>151</v>
       </c>
       <c r="M257" t="s">
         <v>121</v>
@@ -6947,19 +6970,16 @@
         <v>77</v>
       </c>
       <c r="B258" t="s">
-        <v>112</v>
+        <v>152</v>
       </c>
       <c r="C258" t="s">
         <v>9</v>
       </c>
-      <c r="K258" t="s">
-        <v>39</v>
-      </c>
       <c r="L258" t="s">
-        <v>112</v>
+        <v>152</v>
       </c>
       <c r="M258" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="259" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6967,16 +6987,13 @@
         <v>77</v>
       </c>
       <c r="B259" t="s">
-        <v>113</v>
+        <v>153</v>
       </c>
       <c r="C259" t="s">
-        <v>9</v>
-      </c>
-      <c r="J259" t="s">
-        <v>431</v>
+        <v>17</v>
       </c>
       <c r="L259" t="s">
-        <v>113</v>
+        <v>153</v>
       </c>
       <c r="M259" t="s">
         <v>121</v>
@@ -6987,16 +7004,19 @@
         <v>77</v>
       </c>
       <c r="B260" t="s">
-        <v>206</v>
+        <v>405</v>
       </c>
       <c r="C260" t="s">
-        <v>52</v>
+        <v>9</v>
+      </c>
+      <c r="K260" t="s">
+        <v>385</v>
       </c>
       <c r="L260" t="s">
-        <v>206</v>
+        <v>405</v>
       </c>
       <c r="M260" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="261" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7004,22 +7024,19 @@
         <v>77</v>
       </c>
       <c r="B261" t="s">
-        <v>206</v>
+        <v>112</v>
       </c>
       <c r="C261" t="s">
-        <v>15</v>
-      </c>
-      <c r="D261" t="s">
-        <v>308</v>
-      </c>
-      <c r="J261" t="s">
-        <v>438</v>
+        <v>9</v>
+      </c>
+      <c r="K261" t="s">
+        <v>39</v>
       </c>
       <c r="L261" t="s">
-        <v>226</v>
-      </c>
-      <c r="M261" s="1" t="s">
-        <v>245</v>
+        <v>112</v>
+      </c>
+      <c r="M261" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="262" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7027,16 +7044,19 @@
         <v>77</v>
       </c>
       <c r="B262" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
       <c r="C262" t="s">
         <v>9</v>
       </c>
+      <c r="J262" t="s">
+        <v>431</v>
+      </c>
       <c r="L262" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
       <c r="M262" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="263" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7044,16 +7064,16 @@
         <v>77</v>
       </c>
       <c r="B263" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="C263" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="L263" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="M263" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="264" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7061,16 +7081,22 @@
         <v>77</v>
       </c>
       <c r="B264" t="s">
-        <v>380</v>
+        <v>206</v>
       </c>
       <c r="C264" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="D264" t="s">
+        <v>308</v>
+      </c>
+      <c r="J264" t="s">
+        <v>438</v>
       </c>
       <c r="L264" t="s">
-        <v>380</v>
-      </c>
-      <c r="M264" t="s">
-        <v>125</v>
+        <v>226</v>
+      </c>
+      <c r="M264" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="265" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7078,19 +7104,16 @@
         <v>77</v>
       </c>
       <c r="B265" t="s">
-        <v>381</v>
+        <v>148</v>
       </c>
       <c r="C265" t="s">
-        <v>15</v>
-      </c>
-      <c r="H265" t="s">
-        <v>382</v>
+        <v>9</v>
       </c>
       <c r="L265" t="s">
-        <v>381</v>
+        <v>148</v>
       </c>
       <c r="M265" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="266" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7098,16 +7121,16 @@
         <v>77</v>
       </c>
       <c r="B266" t="s">
-        <v>383</v>
+        <v>190</v>
       </c>
       <c r="C266" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="L266" t="s">
-        <v>383</v>
+        <v>190</v>
       </c>
       <c r="M266" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="267" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7115,85 +7138,76 @@
         <v>77</v>
       </c>
       <c r="B267" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C267" t="s">
-        <v>15</v>
-      </c>
-      <c r="D267" t="s">
-        <v>308</v>
-      </c>
-      <c r="J267" t="s">
-        <v>438</v>
+        <v>9</v>
       </c>
       <c r="L267" t="s">
-        <v>384</v>
-      </c>
-      <c r="M267" s="1" t="s">
-        <v>245</v>
+        <v>380</v>
+      </c>
+      <c r="M267" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="268" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>114</v>
+        <v>77</v>
       </c>
       <c r="B268" t="s">
-        <v>115</v>
+        <v>381</v>
       </c>
       <c r="C268" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="H268" t="s">
+        <v>382</v>
       </c>
       <c r="L268" t="s">
-        <v>115</v>
+        <v>381</v>
       </c>
       <c r="M268" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="269" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>114</v>
+        <v>77</v>
       </c>
       <c r="B269" t="s">
-        <v>116</v>
+        <v>383</v>
       </c>
       <c r="C269" t="s">
-        <v>9</v>
-      </c>
-      <c r="D269" t="s">
-        <v>305</v>
-      </c>
-      <c r="F269" t="s">
-        <v>11</v>
-      </c>
-      <c r="H269" t="s">
-        <v>448</v>
-      </c>
-      <c r="I269" t="s">
-        <v>447</v>
+        <v>52</v>
       </c>
       <c r="L269" t="s">
-        <v>116</v>
+        <v>383</v>
       </c>
       <c r="M269" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
     </row>
     <row r="270" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>114</v>
+        <v>77</v>
       </c>
       <c r="B270" t="s">
-        <v>117</v>
+        <v>383</v>
       </c>
       <c r="C270" t="s">
         <v>15</v>
       </c>
+      <c r="D270" t="s">
+        <v>308</v>
+      </c>
+      <c r="J270" t="s">
+        <v>438</v>
+      </c>
       <c r="L270" t="s">
-        <v>117</v>
-      </c>
-      <c r="M270" t="s">
-        <v>122</v>
+        <v>384</v>
+      </c>
+      <c r="M270" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="271" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7201,16 +7215,16 @@
         <v>114</v>
       </c>
       <c r="B271" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C271" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="L271" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="M271" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="272" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7218,16 +7232,28 @@
         <v>114</v>
       </c>
       <c r="B272" t="s">
-        <v>446</v>
+        <v>116</v>
       </c>
       <c r="C272" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="D272" t="s">
+        <v>305</v>
+      </c>
+      <c r="F272" t="s">
+        <v>11</v>
+      </c>
+      <c r="H272" t="s">
+        <v>448</v>
+      </c>
+      <c r="I272" t="s">
+        <v>447</v>
       </c>
       <c r="L272" t="s">
-        <v>446</v>
+        <v>116</v>
       </c>
       <c r="M272" t="s">
-        <v>121</v>
+        <v>149</v>
       </c>
     </row>
     <row r="273" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7235,19 +7261,16 @@
         <v>114</v>
       </c>
       <c r="B273" t="s">
-        <v>440</v>
+        <v>117</v>
       </c>
       <c r="C273" t="s">
-        <v>9</v>
-      </c>
-      <c r="K273" t="s">
-        <v>114</v>
+        <v>15</v>
       </c>
       <c r="L273" t="s">
-        <v>440</v>
+        <v>117</v>
       </c>
       <c r="M273" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="274" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7255,13 +7278,13 @@
         <v>114</v>
       </c>
       <c r="B274" t="s">
-        <v>406</v>
+        <v>118</v>
       </c>
       <c r="C274" t="s">
         <v>17</v>
       </c>
       <c r="L274" t="s">
-        <v>406</v>
+        <v>118</v>
       </c>
       <c r="M274" t="s">
         <v>121</v>
@@ -7272,13 +7295,13 @@
         <v>114</v>
       </c>
       <c r="B275" t="s">
-        <v>411</v>
+        <v>446</v>
       </c>
       <c r="C275" t="s">
         <v>17</v>
       </c>
       <c r="L275" t="s">
-        <v>411</v>
+        <v>446</v>
       </c>
       <c r="M275" t="s">
         <v>121</v>
@@ -7289,16 +7312,19 @@
         <v>114</v>
       </c>
       <c r="B276" t="s">
-        <v>268</v>
+        <v>440</v>
       </c>
       <c r="C276" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="K276" t="s">
+        <v>114</v>
       </c>
       <c r="L276" t="s">
-        <v>268</v>
+        <v>440</v>
       </c>
       <c r="M276" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="277" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7306,25 +7332,13 @@
         <v>114</v>
       </c>
       <c r="B277" t="s">
-        <v>196</v>
+        <v>406</v>
       </c>
       <c r="C277" t="s">
-        <v>15</v>
-      </c>
-      <c r="D277" t="s">
-        <v>329</v>
-      </c>
-      <c r="E277" t="s">
-        <v>199</v>
-      </c>
-      <c r="F277" t="s">
-        <v>195</v>
-      </c>
-      <c r="G277" t="s">
-        <v>200</v>
+        <v>17</v>
       </c>
       <c r="L277" t="s">
-        <v>196</v>
+        <v>406</v>
       </c>
       <c r="M277" t="s">
         <v>121</v>
@@ -7335,13 +7349,13 @@
         <v>114</v>
       </c>
       <c r="B278" t="s">
-        <v>197</v>
+        <v>411</v>
       </c>
       <c r="C278" t="s">
         <v>17</v>
       </c>
       <c r="L278" t="s">
-        <v>197</v>
+        <v>411</v>
       </c>
       <c r="M278" t="s">
         <v>121</v>
@@ -7352,16 +7366,16 @@
         <v>114</v>
       </c>
       <c r="B279" t="s">
-        <v>198</v>
+        <v>268</v>
       </c>
       <c r="C279" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="L279" t="s">
-        <v>198</v>
+        <v>268</v>
       </c>
       <c r="M279" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="280" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7369,22 +7383,28 @@
         <v>114</v>
       </c>
       <c r="B280" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C280" t="s">
         <v>15</v>
       </c>
       <c r="D280" t="s">
-        <v>308</v>
-      </c>
-      <c r="J280" t="s">
-        <v>438</v>
+        <v>329</v>
+      </c>
+      <c r="E280" t="s">
+        <v>199</v>
+      </c>
+      <c r="F280" t="s">
+        <v>195</v>
+      </c>
+      <c r="G280" t="s">
+        <v>200</v>
       </c>
       <c r="L280" t="s">
-        <v>225</v>
-      </c>
-      <c r="M280" s="1" t="s">
-        <v>245</v>
+        <v>196</v>
+      </c>
+      <c r="M280" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="281" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7392,16 +7412,13 @@
         <v>114</v>
       </c>
       <c r="B281" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C281" t="s">
-        <v>9</v>
-      </c>
-      <c r="K281" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L281" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="M281" t="s">
         <v>121</v>
@@ -7412,22 +7429,16 @@
         <v>114</v>
       </c>
       <c r="B282" t="s">
-        <v>407</v>
+        <v>198</v>
       </c>
       <c r="C282" t="s">
-        <v>9</v>
-      </c>
-      <c r="D282" t="s">
-        <v>310</v>
-      </c>
-      <c r="J282" t="s">
-        <v>416</v>
+        <v>52</v>
       </c>
       <c r="L282" t="s">
-        <v>407</v>
+        <v>198</v>
       </c>
       <c r="M282" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="283" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7435,85 +7446,88 @@
         <v>114</v>
       </c>
       <c r="B283" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="C283" t="s">
         <v>15</v>
       </c>
       <c r="D283" t="s">
-        <v>330</v>
+        <v>308</v>
       </c>
       <c r="J283" t="s">
-        <v>432</v>
+        <v>438</v>
       </c>
       <c r="L283" t="s">
-        <v>216</v>
-      </c>
-      <c r="M283" t="s">
-        <v>121</v>
+        <v>225</v>
+      </c>
+      <c r="M283" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="284" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>385</v>
+        <v>114</v>
       </c>
       <c r="B284" t="s">
-        <v>386</v>
+        <v>207</v>
       </c>
       <c r="C284" t="s">
         <v>9</v>
       </c>
+      <c r="K284" t="s">
+        <v>20</v>
+      </c>
       <c r="L284" t="s">
-        <v>386</v>
+        <v>207</v>
       </c>
       <c r="M284" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="285" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>385</v>
+        <v>114</v>
       </c>
       <c r="B285" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="C285" t="s">
         <v>9</v>
       </c>
       <c r="D285" t="s">
-        <v>305</v>
-      </c>
-      <c r="F285" t="s">
-        <v>11</v>
-      </c>
-      <c r="H285" t="s">
-        <v>448</v>
-      </c>
-      <c r="I285" t="s">
-        <v>447</v>
+        <v>310</v>
+      </c>
+      <c r="J285" t="s">
+        <v>416</v>
       </c>
       <c r="L285" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="M285" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
     </row>
     <row r="286" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>385</v>
+        <v>114</v>
       </c>
       <c r="B286" t="s">
-        <v>387</v>
+        <v>216</v>
       </c>
       <c r="C286" t="s">
         <v>15</v>
       </c>
+      <c r="D286" t="s">
+        <v>330</v>
+      </c>
+      <c r="J286" t="s">
+        <v>432</v>
+      </c>
       <c r="L286" t="s">
-        <v>387</v>
+        <v>216</v>
       </c>
       <c r="M286" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="287" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7521,16 +7535,16 @@
         <v>385</v>
       </c>
       <c r="B287" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C287" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="L287" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="M287" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="288" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7538,22 +7552,28 @@
         <v>385</v>
       </c>
       <c r="B288" t="s">
-        <v>388</v>
+        <v>403</v>
       </c>
       <c r="C288" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D288" t="s">
-        <v>308</v>
-      </c>
-      <c r="J288" t="s">
-        <v>438</v>
+        <v>305</v>
+      </c>
+      <c r="F288" t="s">
+        <v>11</v>
+      </c>
+      <c r="H288" t="s">
+        <v>448</v>
+      </c>
+      <c r="I288" t="s">
+        <v>447</v>
       </c>
       <c r="L288" t="s">
-        <v>389</v>
-      </c>
-      <c r="M288" s="1" t="s">
-        <v>245</v>
+        <v>403</v>
+      </c>
+      <c r="M288" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="289" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7561,22 +7581,16 @@
         <v>385</v>
       </c>
       <c r="B289" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C289" t="s">
-        <v>9</v>
-      </c>
-      <c r="D289" t="s">
-        <v>435</v>
-      </c>
-      <c r="J289" t="s">
-        <v>433</v>
+        <v>15</v>
       </c>
       <c r="L289" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="M289" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="290" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7584,22 +7598,16 @@
         <v>385</v>
       </c>
       <c r="B290" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C290" t="s">
-        <v>9</v>
-      </c>
-      <c r="D290" t="s">
-        <v>436</v>
-      </c>
-      <c r="J290" t="s">
-        <v>434</v>
+        <v>52</v>
       </c>
       <c r="L290" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="M290" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="291" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7607,19 +7615,22 @@
         <v>385</v>
       </c>
       <c r="B291" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C291" t="s">
-        <v>9</v>
-      </c>
-      <c r="K291" t="s">
-        <v>39</v>
+        <v>15</v>
+      </c>
+      <c r="D291" t="s">
+        <v>308</v>
+      </c>
+      <c r="J291" t="s">
+        <v>438</v>
       </c>
       <c r="L291" t="s">
-        <v>392</v>
-      </c>
-      <c r="M291" t="s">
-        <v>121</v>
+        <v>389</v>
+      </c>
+      <c r="M291" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="292" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7627,16 +7638,19 @@
         <v>385</v>
       </c>
       <c r="B292" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C292" t="s">
         <v>9</v>
       </c>
+      <c r="D292" t="s">
+        <v>435</v>
+      </c>
       <c r="J292" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="L292" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="M292" t="s">
         <v>121</v>
@@ -7647,25 +7661,19 @@
         <v>385</v>
       </c>
       <c r="B293" t="s">
-        <v>450</v>
+        <v>391</v>
       </c>
       <c r="C293" t="s">
         <v>9</v>
       </c>
       <c r="D293" t="s">
-        <v>451</v>
-      </c>
-      <c r="F293" t="s">
-        <v>11</v>
-      </c>
-      <c r="H293" t="s">
-        <v>452</v>
-      </c>
-      <c r="I293" t="s">
-        <v>453</v>
+        <v>436</v>
+      </c>
+      <c r="J293" t="s">
+        <v>434</v>
       </c>
       <c r="L293" t="s">
-        <v>450</v>
+        <v>391</v>
       </c>
       <c r="M293" t="s">
         <v>121</v>
@@ -7676,16 +7684,19 @@
         <v>385</v>
       </c>
       <c r="B294" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C294" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="K294" t="s">
+        <v>39</v>
       </c>
       <c r="L294" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="M294" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="295" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7693,16 +7704,19 @@
         <v>385</v>
       </c>
       <c r="B295" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C295" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="J295" t="s">
+        <v>431</v>
       </c>
       <c r="L295" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="M295" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="296" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7710,16 +7724,25 @@
         <v>385</v>
       </c>
       <c r="B296" t="s">
-        <v>396</v>
+        <v>450</v>
       </c>
       <c r="C296" t="s">
-        <v>15</v>
-      </c>
-      <c r="J296" t="s">
-        <v>437</v>
+        <v>9</v>
+      </c>
+      <c r="D296" t="s">
+        <v>451</v>
+      </c>
+      <c r="F296" t="s">
+        <v>11</v>
+      </c>
+      <c r="H296" t="s">
+        <v>452</v>
+      </c>
+      <c r="I296" t="s">
+        <v>453</v>
       </c>
       <c r="L296" t="s">
-        <v>396</v>
+        <v>450</v>
       </c>
       <c r="M296" t="s">
         <v>121</v>
@@ -7730,13 +7753,13 @@
         <v>385</v>
       </c>
       <c r="B297" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C297" t="s">
         <v>15</v>
       </c>
       <c r="L297" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="M297" t="s">
         <v>122</v>
@@ -7747,16 +7770,16 @@
         <v>385</v>
       </c>
       <c r="B298" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C298" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L298" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="M298" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="299" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7764,13 +7787,16 @@
         <v>385</v>
       </c>
       <c r="B299" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C299" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="J299" t="s">
+        <v>437</v>
       </c>
       <c r="L299" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="M299" t="s">
         <v>121</v>
@@ -7781,16 +7807,16 @@
         <v>385</v>
       </c>
       <c r="B300" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C300" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L300" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="M300" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="301" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7798,16 +7824,16 @@
         <v>385</v>
       </c>
       <c r="B301" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C301" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="L301" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="M301" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="302" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7815,18 +7841,69 @@
         <v>385</v>
       </c>
       <c r="B302" t="s">
+        <v>399</v>
+      </c>
+      <c r="C302" t="s">
+        <v>17</v>
+      </c>
+      <c r="L302" t="s">
+        <v>399</v>
+      </c>
+      <c r="M302" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="303" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>385</v>
+      </c>
+      <c r="B303" t="s">
+        <v>400</v>
+      </c>
+      <c r="C303" t="s">
+        <v>17</v>
+      </c>
+      <c r="L303" t="s">
+        <v>400</v>
+      </c>
+      <c r="M303" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="304" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>385</v>
+      </c>
+      <c r="B304" t="s">
+        <v>401</v>
+      </c>
+      <c r="C304" t="s">
+        <v>9</v>
+      </c>
+      <c r="L304" t="s">
+        <v>401</v>
+      </c>
+      <c r="M304" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="305" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>385</v>
+      </c>
+      <c r="B305" t="s">
         <v>402</v>
       </c>
-      <c r="C302" t="s">
-        <v>9</v>
-      </c>
-      <c r="K302" t="s">
-        <v>77</v>
-      </c>
-      <c r="L302" t="s">
+      <c r="C305" t="s">
+        <v>9</v>
+      </c>
+      <c r="K305" t="s">
+        <v>77</v>
+      </c>
+      <c r="L305" t="s">
         <v>402</v>
       </c>
-      <c r="M302" t="s">
+      <c r="M305" t="s">
         <v>121</v>
       </c>
     </row>

</xml_diff>